<commit_message>
final version in IEMCON#
</commit_message>
<xml_diff>
--- a/experiments/counting.xlsx
+++ b/experiments/counting.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="threshold" sheetId="1" r:id="rId1"/>
@@ -40,18 +40,6 @@
     <t>auto</t>
   </si>
   <si>
-    <t>rgb</t>
-  </si>
-  <si>
-    <t>channel red</t>
-  </si>
-  <si>
-    <t>hsv channel 1</t>
-  </si>
-  <si>
-    <t>hed color space</t>
-  </si>
-  <si>
     <t>the kernel size of the bilateral filter</t>
   </si>
   <si>
@@ -62,6 +50,18 @@
   </si>
   <si>
     <t>without the Canny edge detector</t>
+  </si>
+  <si>
+    <t>HED</t>
+  </si>
+  <si>
+    <t>HSV</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Grayscale</t>
   </si>
 </sst>
 </file>
@@ -350,11 +350,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2118514416"/>
-        <c:axId val="-2118522352"/>
+        <c:axId val="2110731952"/>
+        <c:axId val="-2145469104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2118514416"/>
+        <c:axId val="2110731952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -397,7 +397,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2118522352"/>
+        <c:crossAx val="-2145469104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -405,7 +405,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2118522352"/>
+        <c:axId val="-2145469104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -456,7 +456,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2118514416"/>
+        <c:crossAx val="2110731952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -733,11 +733,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2118418160"/>
-        <c:axId val="-2118414720"/>
+        <c:axId val="2109765968"/>
+        <c:axId val="2109762576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2118418160"/>
+        <c:axId val="2109765968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -780,7 +780,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2118414720"/>
+        <c:crossAx val="2109762576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -788,7 +788,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2118414720"/>
+        <c:axId val="2109762576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -839,7 +839,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2118418160"/>
+        <c:crossAx val="2109765968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1028,11 +1028,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2118373840"/>
-        <c:axId val="-2118370464"/>
+        <c:axId val="-2145423152"/>
+        <c:axId val="-2145419776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2118373840"/>
+        <c:axId val="-2145423152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1075,7 +1075,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2118370464"/>
+        <c:crossAx val="-2145419776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1083,7 +1083,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2118370464"/>
+        <c:axId val="-2145419776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1134,7 +1134,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2118373840"/>
+        <c:crossAx val="-2145423152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1263,11 +1263,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2118323456"/>
-        <c:axId val="-2118320016"/>
+        <c:axId val="2110762096"/>
+        <c:axId val="2109776560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2118323456"/>
+        <c:axId val="2110762096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1310,7 +1310,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2118320016"/>
+        <c:crossAx val="2109776560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1318,7 +1318,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2118320016"/>
+        <c:axId val="2109776560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1369,7 +1369,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2118323456"/>
+        <c:crossAx val="2110762096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1432,67 +1432,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>The performance</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of the framework using different color space</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -1500,9 +1440,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.0834142607174103"/>
-          <c:y val="0.21337962962963"/>
+          <c:y val="0.0520039161771445"/>
           <c:w val="0.883252405949256"/>
-          <c:h val="0.700054316127151"/>
+          <c:h val="0.861430029579636"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1528,16 +1468,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>hed color space</c:v>
+                  <c:v>HED</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>rgb</c:v>
+                  <c:v>Grayscale</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>channel red</c:v>
+                  <c:v>Red</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>hsv channel 1</c:v>
+                  <c:v>HSV</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1574,11 +1514,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2119202032"/>
-        <c:axId val="-2119198640"/>
+        <c:axId val="-2143200336"/>
+        <c:axId val="-2143196944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2119202032"/>
+        <c:axId val="-2143200336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1621,7 +1561,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2119198640"/>
+        <c:crossAx val="-2143196944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1629,7 +1569,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2119198640"/>
+        <c:axId val="-2143196944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1680,7 +1620,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2119202032"/>
+        <c:crossAx val="-2143200336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4474,16 +4414,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>650421</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>122918</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>412295</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>168276</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>805089</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>20411</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>566963</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>65768</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4614,16 +4554,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4910,7 +4850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" zoomScalePageLayoutView="112" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScale="112" zoomScaleNormal="112" zoomScalePageLayoutView="112" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -5034,7 +4974,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5049,7 +4991,7 @@
         <v>88.67</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -5303,7 +5245,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1">
         <v>90.99</v>
@@ -5311,7 +5253,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
         <v>87.02</v>
@@ -5319,7 +5261,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>79.02</v>
@@ -5335,15 +5277,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1">
         <v>90.37</v>
@@ -5351,7 +5293,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>83.75</v>
@@ -5359,7 +5301,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>61.4</v>
@@ -5367,7 +5309,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>55.44</v>

</xml_diff>